<commit_message>
Maquilador, back end, bug de indicaciones
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/Maquilador/MaquiladorListado.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/Maquilador/MaquiladorListado.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\API\Service.Catalog\wwwroot\layout\excel\Indicaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\API\Service.Catalog\wwwroot\layout\excel\Maquilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83DB0D4-42CB-4157-A0A6-9D470DC337FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7626FF4E-C831-427A-86A5-FA47F2B9BF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Indicaciones" sheetId="1" r:id="rId1"/>
+    <sheet name="Maquilador" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Indicaciones">Indicaciones!$A$4:$D$5</definedName>
+    <definedName name="Maquilador">Maquilador!$A$4:$F$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Clave</t>
   </si>
@@ -92,13 +92,25 @@
     </r>
   </si>
   <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>{{item.Descripcion}}</t>
-  </si>
-  <si>
     <t>{{item.Nombre}}</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>{{item.Direccion}}</t>
+  </si>
+  <si>
+    <t>{{item.Correo}}</t>
+  </si>
+  <si>
+    <t>{{item.Telefono}}</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>Dirección</t>
   </si>
 </sst>
 </file>
@@ -173,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,6 +196,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,15 +572,15 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
   </cols>
@@ -577,8 +592,8 @@
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
@@ -590,25 +605,36 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -617,7 +643,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>